<commit_message>
Updated TestMatrix, added mean image code
</commit_message>
<xml_diff>
--- a/TestMatrix.xlsx
+++ b/TestMatrix.xlsx
@@ -45,12 +45,6 @@
     <t>Testing Matrix</t>
   </si>
   <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>AlexNet</t>
-  </si>
-  <si>
     <t>GoogLeNet Cars</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>15K, 30K</t>
+  </si>
+  <si>
+    <t>Crop Size</t>
+  </si>
+  <si>
+    <t>Flickr</t>
   </si>
 </sst>
 </file>
@@ -125,8 +125,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -145,22 +147,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,19 +497,19 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C9" sqref="C9:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
@@ -524,10 +528,10 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -537,8 +541,8 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D3">
         <v>512</v>
@@ -547,7 +551,10 @@
         <v>0.05</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>496</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -555,7 +562,7 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="5"/>
       <c r="D4">
         <v>512</v>
       </c>
@@ -563,7 +570,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>496</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -571,7 +581,7 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="5"/>
       <c r="D5">
         <v>256</v>
       </c>
@@ -579,7 +589,10 @@
         <v>0.05</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -587,7 +600,7 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="5"/>
       <c r="D6">
         <v>256</v>
       </c>
@@ -595,7 +608,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -603,7 +619,7 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="5"/>
       <c r="D7">
         <v>128</v>
       </c>
@@ -611,7 +627,10 @@
         <v>0.05</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -619,7 +638,7 @@
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="5"/>
       <c r="D8">
         <v>128</v>
       </c>
@@ -627,7 +646,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -637,8 +659,8 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D9">
         <v>512</v>
@@ -647,7 +669,10 @@
         <v>0.05</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>496</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -655,7 +680,7 @@
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="6"/>
       <c r="D10">
         <v>512</v>
       </c>
@@ -663,7 +688,10 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>496</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -671,7 +699,7 @@
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="6"/>
       <c r="D11">
         <v>256</v>
       </c>
@@ -679,7 +707,10 @@
         <v>0.05</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -687,7 +718,7 @@
       <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="6"/>
       <c r="D12">
         <v>256</v>
       </c>
@@ -695,7 +726,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -703,7 +737,7 @@
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="6"/>
       <c r="D13">
         <v>128</v>
       </c>
@@ -711,7 +745,10 @@
         <v>0.05</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -719,7 +756,7 @@
       <c r="B14">
         <v>6</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="6"/>
       <c r="D14">
         <v>128</v>
       </c>
@@ -727,7 +764,10 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>